<commit_message>
initial classes and slots
</commit_message>
<xml_diff>
--- a/project/excel/attributes_of_biosamples.xlsx
+++ b/project/excel/attributes_of_biosamples.xlsx
@@ -4,11 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Biosample" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Biosample1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="BiosampleCollection" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Biosample1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="BiosampleCollection1" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -451,6 +453,32 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>biosamples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>depth</t>
         </is>
       </c>
@@ -458,4 +486,30 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>biosamples</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added outer 'biossamples:' to example
</commit_message>
<xml_diff>
--- a/project/excel/attributes_of_biosamples.xlsx
+++ b/project/excel/attributes_of_biosamples.xlsx
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,11 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>depth</t>
         </is>
@@ -468,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,6 +483,11 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>depth</t>
         </is>

</xml_diff>